<commit_message>
Updated Performance Testing sheet
</commit_message>
<xml_diff>
--- a/docs/PerformanceTesting.xlsx
+++ b/docs/PerformanceTesting.xlsx
@@ -69,7 +69,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -163,11 +163,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,16 +220,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -264,14 +314,14 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="General">
+                <c:pt idx="0">
                   <c:v>129.11011999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>100</c:v>
+                  <c:v>129.11011999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129.11011999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -314,14 +364,14 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>128.11011999999999</c:v>
+                <c:pt idx="0">
+                  <c:v>129.11011999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2" formatCode="General">
-                  <c:v>100</c:v>
+                  <c:v>129.11011999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>129.11011999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -369,7 +419,7 @@
           </c:tx>
           <c:layout/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="97488256"/>
         <c:crosses val="autoZero"/>
@@ -712,8 +762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -771,96 +821,191 @@
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="20">
         <f>129110.12/1000</f>
         <v>129.11011999999999</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="2"/>
+      <c r="C4" s="20">
+        <f>129110.12/1000</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D4" s="16">
+        <f>129110.12/1000</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E4" s="17">
+        <f>129110.12/1000</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F4" s="20">
+        <f t="shared" ref="F4:G4" si="0">129110.12/1000</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G4" s="20">
+        <f t="shared" si="0"/>
+        <v>129.11011999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5">
-        <f t="shared" ref="B5:B8" si="0">129110.12/1000</f>
-        <v>129.11011999999999</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="2"/>
+      <c r="B5" s="20">
+        <f t="shared" ref="B5:G8" si="1">129110.12/1000</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="C5" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D5" s="12">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E5" s="13">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F5" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G5" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="2">
-        <f t="shared" ref="A6:A8" si="1">A5+1</f>
+        <f t="shared" ref="A6:A8" si="2">A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>129.11011999999999</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="2"/>
+      <c r="B6" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="C6" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D6" s="12">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E6" s="13">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F6" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G6" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>129.11011999999999</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="2"/>
+      <c r="B7" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="C7" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D7" s="12">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E7" s="13">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F7" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G7" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
       <c r="A8" s="2">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>129.11011999999999</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="2"/>
+      <c r="B8" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="C8" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E8" s="19">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F8" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G8" s="20">
+        <f t="shared" si="1"/>
+        <v>129.11011999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" thickTop="1">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="21">
         <f>AVERAGE(B4:B8)</f>
         <v>129.11011999999999</v>
       </c>
-      <c r="C9" s="8">
-        <v>128.11011999999999</v>
-      </c>
-      <c r="D9" s="12">
-        <v>100</v>
-      </c>
-      <c r="E9" s="13">
-        <v>100</v>
-      </c>
-      <c r="F9" s="8">
-        <v>100</v>
-      </c>
-      <c r="G9" s="8">
-        <v>100</v>
+      <c r="C9" s="21">
+        <f t="shared" ref="C9:G9" si="3">AVERAGE(C4:C8)</f>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="D9" s="10">
+        <f t="shared" si="3"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="3"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="F9" s="21">
+        <f t="shared" si="3"/>
+        <v>129.11011999999999</v>
+      </c>
+      <c r="G9" s="21">
+        <f t="shared" si="3"/>
+        <v>129.11011999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <f>B9/C9</f>
-        <v>1.0078057845859485</v>
-      </c>
-      <c r="C10" s="10">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
         <f>C9/B9</f>
-        <v>0.99225467376221166</v>
+        <v>1</v>
       </c>
       <c r="D10" s="14">
         <f>D9/E9</f>
@@ -870,17 +1015,17 @@
         <f>E9/D9</f>
         <v>1</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="8">
         <f>F9/G9</f>
         <v>1</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="8">
         <f>G9/F9</f>
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:7">
-      <c r="F16" s="11"/>
+      <c r="F16" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>